<commit_message>
processed all real data
</commit_message>
<xml_diff>
--- a/data/RockCreekCytometrySamples_Feb17.xlsx
+++ b/data/RockCreekCytometrySamples_Feb17.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/KeithSSD/RockCreek/RC_CellCounts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6305A5-4B3C-424D-8CD5-B9B8EE473DEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F616A880-1200-9E48-B74B-713C28569FF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="0" windowWidth="28540" windowHeight="15880" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="232">
   <si>
     <t>protocol</t>
   </si>
@@ -559,9 +559,6 @@
   </si>
   <si>
     <t>Deadline Schedule</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
   <si>
     <t>RC1-BUOY</t>
@@ -1482,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2A43A8-C417-47C5-9C06-B16FAFE2749E}">
   <dimension ref="A1:P192"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="140" workbookViewId="0">
+      <selection activeCell="E187" sqref="E187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1534,10 +1531,6 @@
       <c r="J1" t="s">
         <v>29</v>
       </c>
-      <c r="K1">
-        <f>COUNTA(J2:J191)</f>
-        <v>182</v>
-      </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="40">
@@ -3643,7 +3636,7 @@
         <v>30</v>
       </c>
       <c r="E69" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F69" s="45" t="s">
         <v>39</v>
@@ -3673,7 +3666,7 @@
         <v>30</v>
       </c>
       <c r="E70" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F70" s="45" t="s">
         <v>39</v>
@@ -4669,7 +4662,7 @@
         <v>31</v>
       </c>
       <c r="F103" s="45" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G103" s="45"/>
       <c r="H103" s="45" t="s">
@@ -4699,7 +4692,7 @@
         <v>31</v>
       </c>
       <c r="F104" s="58" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G104" s="45"/>
       <c r="H104" s="45" t="s">
@@ -5010,9 +5003,6 @@
         <v>2</v>
       </c>
       <c r="K114" s="5"/>
-      <c r="L114" t="s">
-        <v>176</v>
-      </c>
       <c r="M114" s="4"/>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.2">
@@ -7181,7 +7171,7 @@
         <v>37</v>
       </c>
       <c r="E186" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F186" t="s">
         <v>37</v>
@@ -7209,7 +7199,7 @@
         <v>37</v>
       </c>
       <c r="E187" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F187" t="s">
         <v>37</v>
@@ -7334,10 +7324,10 @@
         <v>31</v>
       </c>
       <c r="F192" t="s">
+        <v>178</v>
+      </c>
+      <c r="G192" t="s">
         <v>179</v>
-      </c>
-      <c r="G192" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -7382,43 +7372,43 @@
         <v>52</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G1" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="K1" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="L1" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="P1" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="J1" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="P1" s="14" t="s">
+      <c r="Q1" s="14" t="s">
         <v>189</v>
-      </c>
-      <c r="Q1" s="14" t="s">
-        <v>190</v>
       </c>
       <c r="R1" s="14" t="s">
         <v>27</v>
@@ -7429,7 +7419,7 @@
         <v>43745</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C2" t="s">
         <v>80</v>
@@ -7471,13 +7461,13 @@
         <v>18.3834846560889</v>
       </c>
       <c r="P2" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q2" t="s">
         <v>191</v>
       </c>
-      <c r="Q2" t="s">
-        <v>192</v>
-      </c>
       <c r="R2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -7485,7 +7475,7 @@
         <v>43745</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C3" t="s">
         <v>80</v>
@@ -7521,19 +7511,19 @@
         <v>16601.02</v>
       </c>
       <c r="N3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O3">
         <v>28.954709531542299</v>
       </c>
       <c r="P3" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q3" t="s">
         <v>193</v>
       </c>
-      <c r="Q3" t="s">
-        <v>194</v>
-      </c>
       <c r="R3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -7541,7 +7531,7 @@
         <v>43745</v>
       </c>
       <c r="B4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C4" t="s">
         <v>80</v>
@@ -7577,19 +7567,19 @@
         <v>16601.02</v>
       </c>
       <c r="N4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O4">
         <v>14.100984073001401</v>
       </c>
       <c r="P4" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q4" t="s">
         <v>195</v>
       </c>
-      <c r="Q4" t="s">
-        <v>196</v>
-      </c>
       <c r="R4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -7597,7 +7587,7 @@
         <v>43745</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C5" t="s">
         <v>80</v>
@@ -7633,19 +7623,19 @@
         <v>16601.02</v>
       </c>
       <c r="N5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P5" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q5" t="s">
         <v>197</v>
       </c>
-      <c r="Q5" t="s">
-        <v>198</v>
-      </c>
       <c r="R5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -7653,13 +7643,13 @@
         <v>43745</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C6" t="s">
         <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -7695,13 +7685,13 @@
         <v>15.345173792649399</v>
       </c>
       <c r="P6" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q6" t="s">
         <v>207</v>
       </c>
-      <c r="Q6" t="s">
-        <v>208</v>
-      </c>
       <c r="R6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -7709,13 +7699,13 @@
         <v>43745</v>
       </c>
       <c r="B7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C7" t="s">
         <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -7745,19 +7735,19 @@
         <v>16601.02</v>
       </c>
       <c r="N7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P7" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q7" t="s">
         <v>209</v>
       </c>
-      <c r="Q7" t="s">
-        <v>210</v>
-      </c>
       <c r="R7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -7765,13 +7755,13 @@
         <v>43745</v>
       </c>
       <c r="B8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C8" t="s">
         <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -7801,19 +7791,19 @@
         <v>16601.02</v>
       </c>
       <c r="N8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P8" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q8" t="s">
         <v>211</v>
       </c>
-      <c r="Q8" t="s">
-        <v>212</v>
-      </c>
       <c r="R8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -7821,13 +7811,13 @@
         <v>43745</v>
       </c>
       <c r="B9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C9" t="s">
         <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -7857,19 +7847,19 @@
         <v>16601.02</v>
       </c>
       <c r="N9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P9" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q9" t="s">
         <v>213</v>
       </c>
-      <c r="Q9" t="s">
-        <v>214</v>
-      </c>
       <c r="R9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -7877,10 +7867,10 @@
         <v>43745</v>
       </c>
       <c r="B10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D10" t="s">
         <v>48</v>
@@ -7913,19 +7903,19 @@
         <v>16601.02</v>
       </c>
       <c r="N10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P10" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q10" t="s">
         <v>199</v>
       </c>
-      <c r="Q10" t="s">
-        <v>200</v>
-      </c>
       <c r="R10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -7933,10 +7923,10 @@
         <v>43745</v>
       </c>
       <c r="B11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D11" t="s">
         <v>48</v>
@@ -7969,19 +7959,19 @@
         <v>16601.02</v>
       </c>
       <c r="N11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P11" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q11" t="s">
         <v>201</v>
       </c>
-      <c r="Q11" t="s">
-        <v>202</v>
-      </c>
       <c r="R11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -7989,7 +7979,7 @@
         <v>43745</v>
       </c>
       <c r="B12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C12" t="s">
         <v>80</v>
@@ -8025,19 +8015,19 @@
         <v>16601.02</v>
       </c>
       <c r="N12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P12" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q12" t="s">
         <v>203</v>
       </c>
-      <c r="Q12" t="s">
-        <v>204</v>
-      </c>
       <c r="R12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -8045,7 +8035,7 @@
         <v>43745</v>
       </c>
       <c r="B13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C13" t="s">
         <v>80</v>
@@ -8081,19 +8071,19 @@
         <v>16601.02</v>
       </c>
       <c r="N13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P13" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q13" t="s">
         <v>205</v>
       </c>
-      <c r="Q13" t="s">
-        <v>206</v>
-      </c>
       <c r="R13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>